<commit_message>
Updates to xlsx file and create csv from it
</commit_message>
<xml_diff>
--- a/events/events/_event_data_collector.xlsx
+++ b/events/events/_event_data_collector.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patcallahan/Documents/Coding/Open Science Center/lmu-osc.github.io/events/events/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E369A49-054C-1C4C-AEC6-B2D1F6A5E729}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D06FAAB-5F80-5A44-8989-AA54949BB5C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="46960" windowHeight="25560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="38520" windowHeight="23180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$CH$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$CH$122</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="743">
   <si>
     <t>file_paths</t>
   </si>
@@ -2646,14 +2646,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CH123"/>
+  <dimension ref="A1:CH122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="AH42" sqref="AH42"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="174" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="61.83203125" customWidth="1"/>
     <col min="2" max="2" width="139.5" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
   </cols>
@@ -7225,6 +7226,9 @@
       <c r="F115" t="s">
         <v>185</v>
       </c>
+      <c r="H115" t="s">
+        <v>319</v>
+      </c>
       <c r="X115" t="s">
         <v>229</v>
       </c>
@@ -7252,82 +7256,94 @@
     </row>
     <row r="116" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>314</v>
+        <v>697</v>
       </c>
       <c r="B116" t="s">
-        <v>282</v>
+        <v>698</v>
       </c>
       <c r="C116" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
       <c r="D116" t="s">
-        <v>315</v>
+        <v>699</v>
       </c>
       <c r="E116" t="s">
-        <v>315</v>
-      </c>
-      <c r="F116" t="s">
-        <v>185</v>
-      </c>
-      <c r="H116" t="s">
-        <v>319</v>
-      </c>
+        <v>699</v>
+      </c>
+      <c r="AN116" t="s">
+        <v>700</v>
+      </c>
+      <c r="AP116" t="s">
+        <v>701</v>
+      </c>
+      <c r="AR116" t="s">
+        <v>702</v>
+      </c>
+      <c r="AT116" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AU116" s="3"/>
       <c r="BH116" t="s">
-        <v>257</v>
-      </c>
-      <c r="BJ116" t="s">
-        <v>230</v>
-      </c>
-      <c r="BR116" t="s">
-        <v>185</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="BR116" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="BS116" s="3"/>
       <c r="CH116" t="s">
-        <v>186</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>697</v>
+        <v>523</v>
       </c>
       <c r="B117" t="s">
-        <v>698</v>
+        <v>524</v>
       </c>
       <c r="C117" t="s">
-        <v>142</v>
+        <v>452</v>
       </c>
       <c r="D117" t="s">
-        <v>699</v>
+        <v>525</v>
       </c>
       <c r="E117" t="s">
-        <v>699</v>
+        <v>525</v>
       </c>
       <c r="AN117" t="s">
-        <v>700</v>
+        <v>526</v>
       </c>
       <c r="AP117" t="s">
-        <v>701</v>
-      </c>
-      <c r="AR117" t="s">
-        <v>702</v>
-      </c>
-      <c r="AT117" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="AU117" s="3"/>
+        <v>455</v>
+      </c>
       <c r="BH117" t="s">
-        <v>86</v>
-      </c>
-      <c r="BR117" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="BS117" s="3"/>
+        <v>454</v>
+      </c>
+      <c r="BR117" t="s">
+        <v>455</v>
+      </c>
+      <c r="BT117" t="s">
+        <v>456</v>
+      </c>
+      <c r="BV117" t="s">
+        <v>253</v>
+      </c>
+      <c r="BX117" t="s">
+        <v>526</v>
+      </c>
+      <c r="BZ117" t="s">
+        <v>527</v>
+      </c>
+      <c r="CB117" t="s">
+        <v>528</v>
+      </c>
       <c r="CH117" t="s">
-        <v>119</v>
+        <v>457</v>
       </c>
     </row>
     <row r="118" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>523</v>
+        <v>560</v>
       </c>
       <c r="B118" t="s">
         <v>524</v>
@@ -7336,13 +7352,13 @@
         <v>452</v>
       </c>
       <c r="D118" t="s">
-        <v>525</v>
+        <v>561</v>
       </c>
       <c r="E118" t="s">
-        <v>525</v>
+        <v>561</v>
       </c>
       <c r="AN118" t="s">
-        <v>526</v>
+        <v>538</v>
       </c>
       <c r="AP118" t="s">
         <v>455</v>
@@ -7366,7 +7382,7 @@
         <v>527</v>
       </c>
       <c r="CB118" t="s">
-        <v>528</v>
+        <v>538</v>
       </c>
       <c r="CH118" t="s">
         <v>457</v>
@@ -7374,7 +7390,7 @@
     </row>
     <row r="119" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="B119" t="s">
         <v>524</v>
@@ -7383,16 +7399,16 @@
         <v>452</v>
       </c>
       <c r="D119" t="s">
-        <v>561</v>
+        <v>592</v>
       </c>
       <c r="E119" t="s">
-        <v>561</v>
+        <v>592</v>
       </c>
       <c r="AN119" t="s">
+        <v>455</v>
+      </c>
+      <c r="AP119" t="s">
         <v>538</v>
-      </c>
-      <c r="AP119" t="s">
-        <v>455</v>
       </c>
       <c r="BH119" t="s">
         <v>454</v>
@@ -7401,19 +7417,19 @@
         <v>455</v>
       </c>
       <c r="BT119" t="s">
-        <v>456</v>
+        <v>527</v>
       </c>
       <c r="BV119" t="s">
-        <v>253</v>
+        <v>538</v>
       </c>
       <c r="BX119" t="s">
-        <v>526</v>
+        <v>549</v>
       </c>
       <c r="BZ119" t="s">
-        <v>527</v>
+        <v>236</v>
       </c>
       <c r="CB119" t="s">
-        <v>538</v>
+        <v>300</v>
       </c>
       <c r="CH119" t="s">
         <v>457</v>
@@ -7421,177 +7437,130 @@
     </row>
     <row r="120" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>591</v>
+        <v>614</v>
       </c>
       <c r="B120" t="s">
-        <v>524</v>
+        <v>615</v>
       </c>
       <c r="C120" t="s">
-        <v>452</v>
+        <v>82</v>
       </c>
       <c r="D120" t="s">
-        <v>592</v>
+        <v>616</v>
       </c>
       <c r="E120" t="s">
-        <v>592</v>
+        <v>616</v>
       </c>
       <c r="AN120" t="s">
-        <v>455</v>
+        <v>209</v>
       </c>
       <c r="AP120" t="s">
-        <v>538</v>
+        <v>617</v>
       </c>
       <c r="BH120" t="s">
-        <v>454</v>
+        <v>618</v>
+      </c>
+      <c r="BJ120" t="s">
+        <v>208</v>
+      </c>
+      <c r="BL120" t="s">
+        <v>619</v>
       </c>
       <c r="BR120" t="s">
-        <v>455</v>
-      </c>
-      <c r="BT120" t="s">
-        <v>527</v>
-      </c>
-      <c r="BV120" t="s">
-        <v>538</v>
-      </c>
-      <c r="BX120" t="s">
-        <v>549</v>
-      </c>
-      <c r="BZ120" t="s">
-        <v>236</v>
-      </c>
-      <c r="CB120" t="s">
-        <v>300</v>
+        <v>211</v>
       </c>
       <c r="CH120" t="s">
-        <v>457</v>
+        <v>212</v>
       </c>
     </row>
     <row r="121" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>614</v>
+        <v>437</v>
       </c>
       <c r="B121" t="s">
-        <v>615</v>
+        <v>438</v>
       </c>
       <c r="C121" t="s">
-        <v>82</v>
+        <v>142</v>
       </c>
       <c r="D121" t="s">
-        <v>616</v>
+        <v>439</v>
       </c>
       <c r="E121" t="s">
-        <v>616</v>
+        <v>439</v>
       </c>
       <c r="AN121" t="s">
-        <v>209</v>
+        <v>118</v>
       </c>
       <c r="AP121" t="s">
-        <v>617</v>
+        <v>147</v>
+      </c>
+      <c r="AR121" t="s">
+        <v>89</v>
+      </c>
+      <c r="AT121" t="s">
+        <v>440</v>
+      </c>
+      <c r="AV121" t="s">
+        <v>146</v>
       </c>
       <c r="BH121" t="s">
-        <v>618</v>
-      </c>
-      <c r="BJ121" t="s">
-        <v>208</v>
-      </c>
-      <c r="BL121" t="s">
-        <v>619</v>
+        <v>96</v>
       </c>
       <c r="BR121" t="s">
-        <v>211</v>
+        <v>147</v>
       </c>
       <c r="CH121" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
     </row>
     <row r="122" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>437</v>
+        <v>213</v>
       </c>
       <c r="B122" t="s">
-        <v>438</v>
+        <v>723</v>
       </c>
       <c r="C122" t="s">
         <v>142</v>
       </c>
       <c r="D122" t="s">
-        <v>439</v>
+        <v>214</v>
       </c>
       <c r="E122" t="s">
-        <v>439</v>
+        <v>214</v>
       </c>
       <c r="AN122" t="s">
-        <v>118</v>
+        <v>215</v>
       </c>
       <c r="AP122" t="s">
-        <v>147</v>
+        <v>216</v>
       </c>
       <c r="AR122" t="s">
+        <v>217</v>
+      </c>
+      <c r="AT122" t="s">
+        <v>218</v>
+      </c>
+      <c r="AV122" t="s">
+        <v>219</v>
+      </c>
+      <c r="AX122" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ122" t="s">
+        <v>174</v>
+      </c>
+      <c r="BH122" t="s">
+        <v>168</v>
+      </c>
+      <c r="BR122" t="s">
         <v>89</v>
       </c>
-      <c r="AT122" t="s">
-        <v>440</v>
-      </c>
-      <c r="AV122" t="s">
-        <v>146</v>
-      </c>
-      <c r="BH122" t="s">
-        <v>96</v>
-      </c>
-      <c r="BR122" t="s">
-        <v>147</v>
+      <c r="BT122" t="s">
+        <v>221</v>
       </c>
       <c r="CH122" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="123" spans="1:86" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>213</v>
-      </c>
-      <c r="B123" t="s">
-        <v>723</v>
-      </c>
-      <c r="C123" t="s">
-        <v>142</v>
-      </c>
-      <c r="D123" t="s">
-        <v>214</v>
-      </c>
-      <c r="E123" t="s">
-        <v>214</v>
-      </c>
-      <c r="AN123" t="s">
-        <v>215</v>
-      </c>
-      <c r="AP123" t="s">
-        <v>216</v>
-      </c>
-      <c r="AR123" t="s">
-        <v>217</v>
-      </c>
-      <c r="AT123" t="s">
-        <v>218</v>
-      </c>
-      <c r="AV123" t="s">
-        <v>219</v>
-      </c>
-      <c r="AX123" t="s">
-        <v>220</v>
-      </c>
-      <c r="AZ123" t="s">
-        <v>174</v>
-      </c>
-      <c r="BH123" t="s">
-        <v>168</v>
-      </c>
-      <c r="BR123" t="s">
-        <v>89</v>
-      </c>
-      <c r="BT123" t="s">
-        <v>221</v>
-      </c>
-      <c r="CH123" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>